<commit_message>
testDoSearch using a data provider completed
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\Selenium_HW_2\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EF91EE1-1B36-43C0-BC04-BF69EC96791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB7B724-0983-41EA-905D-AB9D14BA3F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{63BAD3BA-E091-40CE-9B8C-FA220E697B2E}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,12 +34,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>searchterm</t>
   </si>
   <si>
     <t>women T shirts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoodies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jackets </t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shorts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweatshirts </t>
+  </si>
+  <si>
+    <t>Tees</t>
+  </si>
+  <si>
+    <t>Bras</t>
+  </si>
+  <si>
+    <t>Tanks</t>
   </si>
 </sst>
 </file>
@@ -401,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B44960-F352-4FEA-A342-85F04DC89970}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,6 +445,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
test 3 add to the cart completed
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\Selenium_HW_2\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB7B724-0983-41EA-905D-AB9D14BA3F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F75E4C9-5FDF-4FE9-83CD-7EEFFE72947B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{63BAD3BA-E091-40CE-9B8C-FA220E697B2E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>searchterm</t>
   </si>
@@ -64,13 +64,16 @@
   </si>
   <si>
     <t>Tanks</t>
+  </si>
+  <si>
+    <t>Pullover</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +86,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,11 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B44960-F352-4FEA-A342-85F04DC89970}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -485,6 +495,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>